<commit_message>
Mejoras a AddRegistro y simplificación de ventanas
</commit_message>
<xml_diff>
--- a/base_datos_salud_procesada.xlsx
+++ b/base_datos_salud_procesada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3980,6 +3980,41 @@
         <v>66.2471</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>col</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D102" t="n">
+        <v>5</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Medio</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>820.5</v>
+      </c>
+      <c r="G102" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="H102" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="I102" t="n">
+        <v>77.09999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizo AddRegistro y optimizo ventanas
</commit_message>
<xml_diff>
--- a/base_datos_salud_procesada.xlsx
+++ b/base_datos_salud_procesada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4015,6 +4015,42 @@
         <v>77.09999999999999</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D103" t="n">
+        <v>3</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alto
+</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>1500.2</v>
+      </c>
+      <c r="G103" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="H103" t="n">
+        <v>23</v>
+      </c>
+      <c r="I103" t="n">
+        <v>83.40000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>